<commit_message>
updated github links for all teams
</commit_message>
<xml_diff>
--- a/projects/teams.xlsx
+++ b/projects/teams.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C5603-576B-43A8-A610-EE930245F100}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E698C40-CD63-4151-84C3-3E3D4B63091E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Project</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>Chris Martinez</t>
+  </si>
+  <si>
+    <t>https://github.com/gpawell/OtterSpotter</t>
+  </si>
+  <si>
+    <t>https://github.com/daviddahlb/AugmentedRealityGame</t>
+  </si>
+  <si>
+    <t>https://github.com/dhs43/queuehub</t>
+  </si>
+  <si>
+    <t>https://github.com/chriscatzin/RampArt</t>
   </si>
 </sst>
 </file>
@@ -438,7 +450,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -476,6 +488,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
@@ -507,6 +522,9 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -535,6 +553,9 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
@@ -548,12 +569,19 @@
       </c>
       <c r="D7" t="s">
         <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{D4FC6F9C-7D58-4840-BF5A-F05A045BE36D}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{CF407EE7-F022-4CC5-8574-FE9E06E66FED}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{A00B506F-3663-4AD1-8290-91300E9F0BC1}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{C046146A-19B0-4FD6-AFAA-02F367CB96CE}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{361854C9-B6D9-4101-82B3-1F0A98BAA6E1}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{11A70BB2-45A3-4A81-A06C-9BBBB8B30748}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added additional team repos.
</commit_message>
<xml_diff>
--- a/projects/teams.xlsx
+++ b/projects/teams.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E467943E-CC2C-4067-826B-27867892E52A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F6327F-51AB-49BC-BD99-016A083EC252}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2931" yWindow="2923" windowWidth="10458" windowHeight="8391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Project</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>https://github.com/MysticalLatios/RogueTilt</t>
+  </si>
+  <si>
+    <t>https://github.com/MJMG93/RampArt</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -462,9 +465,10 @@
     <col min="2" max="2" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.23046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.921875" customWidth="1"/>
+    <col min="5" max="5" width="21.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -495,7 +499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -512,7 +516,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -529,7 +533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -543,7 +547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -559,8 +563,14 @@
       <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -575,9 +585,6 @@
       </c>
       <c r="E7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -587,8 +594,9 @@
     <hyperlink ref="E7" r:id="rId3" xr:uid="{C046146A-19B0-4FD6-AFAA-02F367CB96CE}"/>
     <hyperlink ref="E4" r:id="rId4" xr:uid="{361854C9-B6D9-4101-82B3-1F0A98BAA6E1}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{11A70BB2-45A3-4A81-A06C-9BBBB8B30748}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{09E6E591-92E6-4ADB-87CC-82E099A26DB2}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{09E6E591-92E6-4ADB-87CC-82E099A26DB2}"/>
     <hyperlink ref="E3" r:id="rId7" xr:uid="{DB343C6D-4AA2-49D6-8E2C-611CFB49F5A8}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{5D19B3D1-5652-4C16-8663-141A99B105C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>